<commit_message>
Uprava Excelu a pridani sloupce ID hrace
</commit_message>
<xml_diff>
--- a/prihlaseni_hraci.xlsx
+++ b/prihlaseni_hraci.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dan\Documents\DAN\ČVUT\OOP\semestralka\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D59EE537-B68E-4E43-AD6D-E7BFB49A385D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{802DE2E0-F960-4008-A46B-520C1BA0E41E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6C8EE765-406C-40AB-A193-14855FF8056C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Přihlášení hráči</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>Nasazení dle žebříčku</t>
+  </si>
+  <si>
+    <t>ID hráče</t>
   </si>
 </sst>
 </file>
@@ -112,11 +115,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -454,7 +458,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -463,7 +467,7 @@
     <col min="2" max="3" width="17.88671875" customWidth="1"/>
     <col min="4" max="4" width="17.77734375" customWidth="1"/>
     <col min="5" max="5" width="17.88671875" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" customWidth="1"/>
+    <col min="6" max="6" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25.8" x14ac:dyDescent="0.5">
@@ -487,7 +491,9 @@
       <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="3"/>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Zrušení sloupce Kategorie a ID Hráče - nepotřebné
</commit_message>
<xml_diff>
--- a/prihlaseni_hraci.xlsx
+++ b/prihlaseni_hraci.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dan\Documents\DAN\ČVUT\OOP\semestralka\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9D46628-8F11-4DAE-B6CF-CB13B89FE615}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15D2159E-028B-4F7D-9974-E9BDBFAE1639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6C8EE765-406C-40AB-A193-14855FF8056C}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6C8EE765-406C-40AB-A193-14855FF8056C}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Přihlášení hráči</t>
   </si>
@@ -47,16 +47,10 @@
     <t>Přijmení</t>
   </si>
   <si>
-    <t>Kategorie</t>
-  </si>
-  <si>
     <t>Klub</t>
   </si>
   <si>
     <t>Nasazení dle žebříčku</t>
-  </si>
-  <si>
-    <t>ID hráče</t>
   </si>
   <si>
     <t>Gender</t>
@@ -118,10 +112,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -461,7 +458,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -486,20 +483,16 @@
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>